<commit_message>
- Re-Arrange working folder. - Added blank py file to calculate the statistics.
</commit_message>
<xml_diff>
--- a/Prova.xlsx
+++ b/Prova.xlsx
@@ -3,15 +3,18 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="Questa_cartella_di_lavoro"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28800" yWindow="500" windowWidth="28800" windowHeight="15980" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28800" yWindow="500" windowWidth="28800" windowHeight="15980" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Operazoni" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Statistiche" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Statistica per azione" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet_Nuovo2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Operazioni" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet_Nuovo1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Statistiche" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Statistica per azione" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sheet_Nuovo" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Operazoni'!$A$1:$A$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Operazioni'!$A$1:$A$91</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
@@ -169,12 +172,12 @@
       <protection locked="1" hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,15 +874,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Foglio1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -994,7 +1015,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NFLX</t>
+          <t>STOCAZZO</t>
         </is>
       </c>
       <c r="B6" s="1" t="n">
@@ -2229,11 +2250,6 @@
       <c r="B81" s="1" t="n"/>
     </row>
     <row r="82" ht="15" customHeight="1"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
     <row r="88">
       <c r="B88" s="1" t="n"/>
       <c r="C88" s="1" t="n"/>
@@ -2250,14 +2266,6 @@
       <c r="B91" s="1" t="n"/>
       <c r="C91" s="3" t="n"/>
     </row>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
   </sheetData>
   <autoFilter ref="A1:A91"/>
   <conditionalFormatting sqref="D40:D62 D92:D1048576 D65:D78 D81:D87">
@@ -2371,7 +2379,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Foglio2">
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2385,7 +2411,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col hidden="1" min="1" max="1"/>
+    <col hidden="1" width="13" customWidth="1" min="1" max="1"/>
     <col width="15.33203125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
@@ -2393,7 +2419,7 @@
     <row r="2" hidden="1"/>
     <row r="3" hidden="1"/>
     <row r="4">
-      <c r="B4" s="21" t="inlineStr">
+      <c r="B4" s="18" t="inlineStr">
         <is>
           <t>Bilancio totale</t>
         </is>
@@ -2407,12 +2433,12 @@
         </is>
       </c>
       <c r="O4" s="11">
-        <f>MAX(Operazoni!D:D)</f>
+        <f>MAX(Operazioni!D:D)</f>
         <v/>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="18" t="inlineStr">
+      <c r="B5" s="21" t="inlineStr">
         <is>
           <t>Totale operazioni</t>
         </is>
@@ -2420,7 +2446,7 @@
       <c r="C5" s="19" t="n"/>
       <c r="D5" s="20" t="n"/>
       <c r="E5" s="11">
-        <f>COUNTIF(Operazoni!D:D,"&lt;999999999999")</f>
+        <f>COUNTIF(Operazioni!D:D,"&lt;999999999999")</f>
         <v/>
       </c>
       <c r="N5" s="11" t="inlineStr">
@@ -2429,12 +2455,12 @@
         </is>
       </c>
       <c r="O5" s="11">
-        <f>MIN(Operazoni!D:D)</f>
+        <f>MIN(Operazioni!D:D)</f>
         <v/>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="18" t="inlineStr">
+      <c r="B6" s="21" t="inlineStr">
         <is>
           <t>NET INCOME</t>
         </is>
@@ -2442,7 +2468,7 @@
       <c r="C6" s="19" t="n"/>
       <c r="D6" s="20" t="n"/>
       <c r="E6" s="8">
-        <f>SUM(Operazoni!D:D)</f>
+        <f>SUM(Operazioni!D:D)</f>
         <v/>
       </c>
       <c r="N6" s="11" t="inlineStr">
@@ -2451,12 +2477,12 @@
         </is>
       </c>
       <c r="O6" s="6">
-        <f>MIN(Operazoni!B:B)</f>
+        <f>MIN(Operazioni!B:B)</f>
         <v/>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="18" t="inlineStr">
+      <c r="B7" s="21" t="inlineStr">
         <is>
           <t>OPERAZIONI IN GUADAGNO</t>
         </is>
@@ -2464,7 +2490,7 @@
       <c r="C7" s="19" t="n"/>
       <c r="D7" s="20" t="n"/>
       <c r="E7" s="5">
-        <f>COUNTIF(Operazoni!D:D,"&gt;0")</f>
+        <f>COUNTIF(Operazioni!D:D,"&gt;0")</f>
         <v/>
       </c>
       <c r="N7" s="11" t="inlineStr">
@@ -2473,12 +2499,12 @@
         </is>
       </c>
       <c r="O7" s="6">
-        <f>MAX(Operazoni!B:B)</f>
+        <f>MAX(Operazioni!B:B)</f>
         <v/>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="18" t="inlineStr">
+      <c r="B8" s="21" t="inlineStr">
         <is>
           <t>OPERAZIONI IN PERDITA</t>
         </is>
@@ -2486,7 +2512,7 @@
       <c r="C8" s="19" t="n"/>
       <c r="D8" s="20" t="n"/>
       <c r="E8" s="4">
-        <f>COUNTIF(Operazoni!D:D,"&lt;0")</f>
+        <f>COUNTIF(Operazioni!D:D,"&lt;0")</f>
         <v/>
       </c>
       <c r="N8" s="11" t="inlineStr">
@@ -2500,7 +2526,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="18" t="inlineStr">
+      <c r="B9" s="21" t="inlineStr">
         <is>
           <t>BATTING AVERAGE [%]</t>
         </is>
@@ -2523,7 +2549,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="18" t="inlineStr">
+      <c r="B10" s="21" t="inlineStr">
         <is>
           <t>WIN</t>
         </is>
@@ -2531,7 +2557,7 @@
       <c r="C10" s="19" t="n"/>
       <c r="D10" s="20" t="n"/>
       <c r="E10" s="9">
-        <f>SUMIF(Operazoni!D:D,"&gt;0")</f>
+        <f>SUMIF(Operazioni!D:D,"&gt;0")</f>
         <v/>
       </c>
       <c r="N10" s="11" t="inlineStr">
@@ -2546,7 +2572,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="18" t="inlineStr">
+      <c r="B11" s="21" t="inlineStr">
         <is>
           <t>LOSS</t>
         </is>
@@ -2554,12 +2580,12 @@
       <c r="C11" s="19" t="n"/>
       <c r="D11" s="20" t="n"/>
       <c r="E11" s="10">
-        <f>SUMIF(Operazoni!D:D,"&lt;0") * -1</f>
+        <f>SUMIF(Operazioni!D:D,"&lt;0") * -1</f>
         <v/>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="18" t="inlineStr">
+      <c r="B12" s="21" t="inlineStr">
         <is>
           <t>AVERAGE WIN</t>
         </is>
@@ -2572,7 +2598,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="18" t="inlineStr">
+      <c r="B13" s="21" t="inlineStr">
         <is>
           <t>AVERAGE LOSS</t>
         </is>
@@ -2585,7 +2611,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="18" t="inlineStr">
+      <c r="B14" s="21" t="inlineStr">
         <is>
           <t>WIN/LOSS</t>
         </is>
@@ -2598,7 +2624,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="21" t="inlineStr">
+      <c r="B19" s="18" t="inlineStr">
         <is>
           <t>Bilancio ultima giornata</t>
         </is>
@@ -2606,10 +2632,10 @@
       <c r="C19" s="19" t="n"/>
       <c r="D19" s="20" t="n"/>
       <c r="E19" s="6">
-        <f>Operazoni!E1</f>
-        <v/>
-      </c>
-      <c r="I19" s="21" t="inlineStr">
+        <f>Operazioni!E1</f>
+        <v/>
+      </c>
+      <c r="I19" s="18" t="inlineStr">
         <is>
           <t>Bilancio Intervallo:</t>
         </is>
@@ -2623,7 +2649,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="18" t="inlineStr">
+      <c r="B20" s="21" t="inlineStr">
         <is>
           <t>Totale operazioni</t>
         </is>
@@ -2631,10 +2657,10 @@
       <c r="C20" s="19" t="n"/>
       <c r="D20" s="20" t="n"/>
       <c r="E20" s="11">
-        <f>COUNTIF(Operazoni!B:B,Operazoni!E1)</f>
-        <v/>
-      </c>
-      <c r="I20" s="18" t="inlineStr">
+        <f>COUNTIF(Operazioni!B:B,Operazioni!E1)</f>
+        <v/>
+      </c>
+      <c r="I20" s="21" t="inlineStr">
         <is>
           <t>Totale operazioni</t>
         </is>
@@ -2648,7 +2674,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="18" t="inlineStr">
+      <c r="B21" s="21" t="inlineStr">
         <is>
           <t>TOTAL AMOUNT</t>
         </is>
@@ -2656,10 +2682,10 @@
       <c r="C21" s="19" t="n"/>
       <c r="D21" s="20" t="n"/>
       <c r="E21" s="8">
-        <f>SUMIF(Operazoni!B:B,Operazoni!E1,Operazoni!D:D)</f>
-        <v/>
-      </c>
-      <c r="I21" s="18" t="inlineStr">
+        <f>SUMIF(Operazioni!B:B,Operazioni!E1,Operazioni!D:D)</f>
+        <v/>
+      </c>
+      <c r="I21" s="21" t="inlineStr">
         <is>
           <t>TOTAL AMOUNT</t>
         </is>
@@ -2673,7 +2699,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="18" t="inlineStr">
+      <c r="B22" s="21" t="inlineStr">
         <is>
           <t>OPERAZIONI IN GUADAGNO</t>
         </is>
@@ -2681,10 +2707,10 @@
       <c r="C22" s="19" t="n"/>
       <c r="D22" s="20" t="n"/>
       <c r="E22" s="5">
-        <f>COUNTIFS(Operazoni!B:B,Operazoni!E1,Operazoni!D:D,"&gt;0")</f>
-        <v/>
-      </c>
-      <c r="I22" s="18" t="inlineStr">
+        <f>COUNTIFS(Operazioni!B:B,Operazioni!E1,Operazioni!D:D,"&gt;0")</f>
+        <v/>
+      </c>
+      <c r="I22" s="21" t="inlineStr">
         <is>
           <t>OPERAZIONI IN GUADAGNO</t>
         </is>
@@ -2698,7 +2724,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="18" t="inlineStr">
+      <c r="B23" s="21" t="inlineStr">
         <is>
           <t>OPERAZIONI IN PERDITA</t>
         </is>
@@ -2706,10 +2732,10 @@
       <c r="C23" s="19" t="n"/>
       <c r="D23" s="20" t="n"/>
       <c r="E23" s="4">
-        <f>COUNTIFS(Operazoni!B:B,Operazoni!E1,Operazoni!D:D,"&lt;0")</f>
-        <v/>
-      </c>
-      <c r="I23" s="18" t="inlineStr">
+        <f>COUNTIFS(Operazioni!B:B,Operazioni!E1,Operazioni!D:D,"&lt;0")</f>
+        <v/>
+      </c>
+      <c r="I23" s="21" t="inlineStr">
         <is>
           <t>OPERAZIONI IN PERDITA</t>
         </is>
@@ -2723,7 +2749,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="18" t="inlineStr">
+      <c r="B24" s="21" t="inlineStr">
         <is>
           <t>BATTING AVERAGE [%]</t>
         </is>
@@ -2734,7 +2760,7 @@
         <f>(E22/E20)*100</f>
         <v/>
       </c>
-      <c r="I24" s="18" t="inlineStr">
+      <c r="I24" s="21" t="inlineStr">
         <is>
           <t>BATTING AVERAGE [%]</t>
         </is>
@@ -2748,7 +2774,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="18" t="inlineStr">
+      <c r="B25" s="21" t="inlineStr">
         <is>
           <t>WIN</t>
         </is>
@@ -2756,10 +2782,10 @@
       <c r="C25" s="19" t="n"/>
       <c r="D25" s="20" t="n"/>
       <c r="E25" s="9">
-        <f>SUMIFS(Operazoni!D:D,Operazoni!B:B,Operazoni!E1,Operazoni!D:D,"&gt;0")</f>
-        <v/>
-      </c>
-      <c r="I25" s="18" t="inlineStr">
+        <f>SUMIFS(Operazioni!D:D,Operazioni!B:B,Operazioni!E1,Operazioni!D:D,"&gt;0")</f>
+        <v/>
+      </c>
+      <c r="I25" s="21" t="inlineStr">
         <is>
           <t>WIN</t>
         </is>
@@ -2773,7 +2799,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="18" t="inlineStr">
+      <c r="B26" s="21" t="inlineStr">
         <is>
           <t>LOSS</t>
         </is>
@@ -2781,10 +2807,10 @@
       <c r="C26" s="19" t="n"/>
       <c r="D26" s="20" t="n"/>
       <c r="E26" s="10">
-        <f>SUMIFS(Operazoni!D:D,Operazoni!B:B,Operazoni!E1,Operazoni!D:D,"&lt;0") *-1</f>
-        <v/>
-      </c>
-      <c r="I26" s="18" t="inlineStr">
+        <f>SUMIFS(Operazioni!D:D,Operazioni!B:B,Operazioni!E1,Operazioni!D:D,"&lt;0") *-1</f>
+        <v/>
+      </c>
+      <c r="I26" s="21" t="inlineStr">
         <is>
           <t>LOSS</t>
         </is>
@@ -2798,7 +2824,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="18" t="inlineStr">
+      <c r="B27" s="21" t="inlineStr">
         <is>
           <t>AVERAGE WIN</t>
         </is>
@@ -2809,7 +2835,7 @@
         <f>E25/E22</f>
         <v/>
       </c>
-      <c r="I27" s="18" t="inlineStr">
+      <c r="I27" s="21" t="inlineStr">
         <is>
           <t>AVERAGE WIN</t>
         </is>
@@ -2823,7 +2849,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="18" t="inlineStr">
+      <c r="B28" s="21" t="inlineStr">
         <is>
           <t>AVERAGE LOSS</t>
         </is>
@@ -2834,7 +2860,7 @@
         <f>E26/E23</f>
         <v/>
       </c>
-      <c r="I28" s="18" t="inlineStr">
+      <c r="I28" s="21" t="inlineStr">
         <is>
           <t>AVERAGE LOSS</t>
         </is>
@@ -2848,7 +2874,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="B29" s="18" t="inlineStr">
+      <c r="B29" s="21" t="inlineStr">
         <is>
           <t>WIN/LOSS</t>
         </is>
@@ -2859,7 +2885,7 @@
         <f>E27/(E28)</f>
         <v/>
       </c>
-      <c r="I29" s="18" t="inlineStr">
+      <c r="I29" s="21" t="inlineStr">
         <is>
           <t>WIN/LOSS</t>
         </is>
@@ -2873,7 +2899,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="B35" s="21" t="inlineStr">
+      <c r="B35" s="18" t="inlineStr">
         <is>
           <t>Bilancio Data:</t>
         </is>
@@ -2885,7 +2911,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="B36" s="18" t="inlineStr">
+      <c r="B36" s="21" t="inlineStr">
         <is>
           <t>Totale operazioni</t>
         </is>
@@ -2893,12 +2919,12 @@
       <c r="C36" s="19" t="n"/>
       <c r="D36" s="20" t="n"/>
       <c r="E36" s="12">
-        <f>COUNTIF(Operazoni!B:B,E35)</f>
+        <f>COUNTIF(Operazioni!B:B,E35)</f>
         <v/>
       </c>
     </row>
     <row r="37">
-      <c r="B37" s="18" t="inlineStr">
+      <c r="B37" s="21" t="inlineStr">
         <is>
           <t>TOTAL AMOUNT</t>
         </is>
@@ -2906,12 +2932,12 @@
       <c r="C37" s="19" t="n"/>
       <c r="D37" s="20" t="n"/>
       <c r="E37" s="13">
-        <f>SUMIF(Operazoni!B:B,E35,Operazoni!D:D)</f>
+        <f>SUMIF(Operazioni!B:B,E35,Operazioni!D:D)</f>
         <v/>
       </c>
     </row>
     <row r="38">
-      <c r="B38" s="18" t="inlineStr">
+      <c r="B38" s="21" t="inlineStr">
         <is>
           <t>OPERAZIONI IN GUADAGNO</t>
         </is>
@@ -2919,12 +2945,12 @@
       <c r="C38" s="19" t="n"/>
       <c r="D38" s="20" t="n"/>
       <c r="E38" s="14">
-        <f>COUNTIFS(Operazoni!B:B,E35,Operazoni!D:D,"&gt;0")</f>
+        <f>COUNTIFS(Operazioni!B:B,E35,Operazioni!D:D,"&gt;0")</f>
         <v/>
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="18" t="inlineStr">
+      <c r="B39" s="21" t="inlineStr">
         <is>
           <t>OPERAZIONI IN PERDITA</t>
         </is>
@@ -2932,12 +2958,12 @@
       <c r="C39" s="19" t="n"/>
       <c r="D39" s="20" t="n"/>
       <c r="E39" s="15">
-        <f>COUNTIFS(Operazoni!B:B,E35,Operazoni!D:D,"&lt;0")</f>
+        <f>COUNTIFS(Operazioni!B:B,E35,Operazioni!D:D,"&lt;0")</f>
         <v/>
       </c>
     </row>
     <row r="40">
-      <c r="B40" s="18" t="inlineStr">
+      <c r="B40" s="21" t="inlineStr">
         <is>
           <t>BATTING AVERAGE [%]</t>
         </is>
@@ -2950,7 +2976,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="B41" s="18" t="inlineStr">
+      <c r="B41" s="21" t="inlineStr">
         <is>
           <t>WIN</t>
         </is>
@@ -2958,12 +2984,12 @@
       <c r="C41" s="19" t="n"/>
       <c r="D41" s="20" t="n"/>
       <c r="E41" s="16">
-        <f>SUMIFS(Operazoni!D:D,Operazoni!B:B,E35,Operazoni!D:D,"&gt;0")</f>
+        <f>SUMIFS(Operazioni!D:D,Operazioni!B:B,E35,Operazioni!D:D,"&gt;0")</f>
         <v/>
       </c>
     </row>
     <row r="42">
-      <c r="B42" s="18" t="inlineStr">
+      <c r="B42" s="21" t="inlineStr">
         <is>
           <t>LOSS</t>
         </is>
@@ -2971,12 +2997,12 @@
       <c r="C42" s="19" t="n"/>
       <c r="D42" s="20" t="n"/>
       <c r="E42" s="17">
-        <f>SUMIFS(Operazoni!D:D,Operazoni!B:B,E35,Operazoni!D:D,"&lt;0") *-1</f>
+        <f>SUMIFS(Operazioni!D:D,Operazioni!B:B,E35,Operazioni!D:D,"&lt;0") *-1</f>
         <v/>
       </c>
     </row>
     <row r="43">
-      <c r="B43" s="18" t="inlineStr">
+      <c r="B43" s="21" t="inlineStr">
         <is>
           <t>AVERAGE WIN</t>
         </is>
@@ -2989,7 +3015,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="B44" s="18" t="inlineStr">
+      <c r="B44" s="21" t="inlineStr">
         <is>
           <t>AVERAGE LOSS</t>
         </is>
@@ -3002,7 +3028,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="B45" s="18" t="inlineStr">
+      <c r="B45" s="21" t="inlineStr">
         <is>
           <t>WIN/LOSS</t>
         </is>
@@ -3016,6 +3042,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B35:D35"/>
@@ -3032,34 +3086,6 @@
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <conditionalFormatting sqref="E6">
     <cfRule type="cellIs" priority="8" operator="lessThan" dxfId="1">
@@ -3089,7 +3115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Foglio3">
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3105,4 +3131,22 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>